<commit_message>
annotations in glucose model fixed
</commit_message>
<xml_diff>
--- a/sbmlutils/examples/models/galactose/galactose_annotations.xlsx
+++ b/sbmlutils/examples/models/galactose/galactose_annotations.xlsx
@@ -86,7 +86,7 @@
     <t>liver</t>
   </si>
   <si>
-    <t>UBERON:2107</t>
+    <t>UBERON:0002107</t>
   </si>
   <si>
     <t>uberon</t>
@@ -1242,8 +1242,8 @@
   </sheetPr>
   <dimension ref="A1:G308"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G164" activeCellId="0" sqref="G164"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>